<commit_message>
CI of Lower bound QP time sheet added, all results finished
</commit_message>
<xml_diff>
--- a/Code/SampleRun_Environment_Solar/100Scens/100_LB_Time_CI.xlsx
+++ b/Code/SampleRun_Environment_Solar/100Scens/100_LB_Time_CI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\A_Uni\HiWi\ArticleSubgradient\Code\SampleRun_Environment_Solar\100Scens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EA3A71-EBFD-40B1-8C66-A95962CCC29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5593D029-6641-4058-9E21-2F08C30C3AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="combined_results_IR_1500"/>
+      <sheetName val="LB_Times"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8916,7 +8918,7 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E21"/>
+      <selection activeCell="C2" sqref="C2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8958,7 +8960,7 @@
         <v>0.01</v>
       </c>
       <c r="C2">
-        <v>-2.2672095377284395E-3</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -8996,7 +8998,7 @@
         <v>0.01</v>
       </c>
       <c r="C3">
-        <v>-1.9680135758694947E-4</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9011,7 +9013,7 @@
       </c>
       <c r="L3">
         <f>SUM(C2:C21)/20</f>
-        <v>-2.4590335134482039E-3</v>
+        <v>4</v>
       </c>
       <c r="N3" t="s">
         <v>12</v>
@@ -9044,7 +9046,7 @@
         <v>0.01</v>
       </c>
       <c r="C4">
-        <v>-9.5275244383140924E-3</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9066,11 +9068,11 @@
       </c>
       <c r="O4">
         <f>L3+(-$G$10)*L7/(SQRT(20))</f>
-        <v>-4.3821424733595741E-3</v>
+        <v>4</v>
       </c>
       <c r="P4">
         <f>L3+$G$10*L7/(SQRT(20))</f>
-        <v>-5.359245535368339E-4</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
@@ -9081,7 +9083,7 @@
         <v>0.01</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9114,7 +9116,7 @@
         <v>0.01</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9140,7 +9142,7 @@
         <v>0.01</v>
       </c>
       <c r="C7">
-        <v>-8.3366392460719821E-4</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9155,7 +9157,7 @@
       </c>
       <c r="L7">
         <f>_xlfn.STDEV.S(C2:C21)</f>
-        <v>4.1090806896783563E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
@@ -9166,7 +9168,7 @@
         <v>0.01</v>
       </c>
       <c r="C8">
-        <v>-4.0496496193853085E-3</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9192,7 +9194,7 @@
         <v>0.01</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9214,7 +9216,7 @@
         <v>0.01</v>
       </c>
       <c r="C10">
-        <v>-6.2594674669053663E-3</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9247,7 +9249,7 @@
         <v>0.01</v>
       </c>
       <c r="C11">
-        <v>7.8989460087878398E-4</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9291,7 +9293,7 @@
         <v>0.01</v>
       </c>
       <c r="C12">
-        <v>-1.8579597569379355E-3</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9328,7 +9330,7 @@
         <v>0.01</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9361,7 +9363,7 @@
         <v>0.01</v>
       </c>
       <c r="C14">
-        <v>2.6899304919114419E-4</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9387,7 +9389,7 @@
         <v>0.01</v>
       </c>
       <c r="C15">
-        <v>-7.6696081573004635E-4</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9413,7 +9415,7 @@
         <v>0.01</v>
       </c>
       <c r="C16">
-        <v>-1.5058779745190229E-2</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9439,7 +9441,7 @@
         <v>0.01</v>
       </c>
       <c r="C17">
-        <v>-1.8290387305716633E-3</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9459,7 +9461,7 @@
         <v>0.01</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9478,7 +9480,7 @@
         <v>0.01</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9498,7 +9500,7 @@
         <v>0.01</v>
       </c>
       <c r="C20">
-        <v>-2.0159128225588491E-4</v>
+        <v>4</v>
       </c>
       <c r="D20">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>
@@ -9517,7 +9519,7 @@
         <v>0.01</v>
       </c>
       <c r="C21">
-        <v>-7.3909112438208845E-3</v>
+        <v>4</v>
       </c>
       <c r="D21">
         <f>[1]!combined_results_IR_1500[[#This Row],[100 Solar IR fixed time]]+167</f>

</xml_diff>